<commit_message>
Adicionado novos componentes que serão utilizados no projeto
</commit_message>
<xml_diff>
--- a/documentos/ListaMaterial.xlsx
+++ b/documentos/ListaMaterial.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>SRF02</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Lista de Materiais</t>
   </si>
@@ -59,9 +56,6 @@
     <t>Leitor de Cartão Micro SD</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>http://www.filipeflop.com/pd-361d0e-modulo-cartao-micro-sd.html</t>
   </si>
   <si>
@@ -71,10 +65,22 @@
     <t>http://www.filipeflop.com/pd-23b0f3-cabo-micro-usb-1-2m-multilaser.html?ct=&amp;p=1&amp;s=1</t>
   </si>
   <si>
-    <t>R$14, 90</t>
-  </si>
-  <si>
     <t>http://www.robotshop.com/en/srf02-ultrasonic-range-finder.html</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Sensor SRF02</t>
+  </si>
+  <si>
+    <t>Sensor HC-SR04</t>
+  </si>
+  <si>
+    <t>http://www.filipeflop.com/pd-6b8a2-sensor-de-distancia-ultrassonico-hc-sr04.html</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -84,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +120,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -129,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -214,21 +228,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -243,25 +297,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,150 +626,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8">
         <v>5</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="16">
+        <v>41.03</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="22">
+        <f>C4*E4</f>
+        <v>205.15</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="18">
+        <v>5</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20">
+        <v>9.9</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22">
+        <f>C5*E5</f>
+        <v>49.5</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="22">
+        <f>C6*E6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="3">
+        <f>C7*E7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="16">
+        <v>14.9</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="22">
+        <f>C8*E8</f>
+        <v>29.8</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="14">
+        <v>22.9</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="22">
+        <f>C9*E9</f>
+        <v>45.8</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5">
-        <v>41.03</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="16">
-        <v>22.9</v>
-      </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="16">
+        <v>12.9</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="22">
+        <f>C10*E10</f>
+        <v>12.9</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5">
-        <v>12.9</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="25">
+        <f>SUM(G4:G10)</f>
+        <v>343.15</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J13" s="2"/>
@@ -707,34 +826,38 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I14" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G16" s="2"/>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A1:G2"/>
+  <mergeCells count="26">
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adicionado mais material que será utilizado no protótipo dos óculos
</commit_message>
<xml_diff>
--- a/documentos/ListaMaterial.xlsx
+++ b/documentos/ListaMaterial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Lista de Materiais</t>
   </si>
@@ -81,16 +81,26 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Sensor PIR</t>
+  </si>
+  <si>
+    <t>http://www.filipeflop.com/pd-6b901-sensor-de-movimento-presenca-pir.html</t>
+  </si>
+  <si>
+    <t>*Links possíveis de serem mudados caso seja encontrado um preço mais barato*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +138,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -143,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -265,15 +282,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -282,9 +310,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -300,40 +355,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,252 +636,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="62.28515625" customWidth="1"/>
+    <col min="8" max="8" width="83" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="5"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="23"/>
+      <c r="G3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11">
         <v>5</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="16">
         <v>41.03</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="22">
-        <f>C4*E4</f>
+      <c r="F4" s="16"/>
+      <c r="G4" s="8">
+        <f t="shared" ref="G4:G11" si="0">C4*E4</f>
         <v>205.15</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="18">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15">
         <v>5</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20">
+      <c r="D5" s="14"/>
+      <c r="E5" s="17">
         <v>9.9</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22">
-        <f>C5*E5</f>
+      <c r="F5" s="18"/>
+      <c r="G5" s="8">
+        <f t="shared" si="0"/>
         <v>49.5</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="22">
-        <f>C6*E6</f>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11">
+        <v>2</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="16">
+        <v>10</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11">
         <v>2</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="3">
-        <f>C7*E7</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="16">
         <v>14.9</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="22">
-        <f>C8*E8</f>
+      <c r="F8" s="16"/>
+      <c r="G8" s="8">
+        <f t="shared" si="0"/>
         <v>29.8</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8">
+      <c r="B9" s="14"/>
+      <c r="C9" s="11">
         <v>2</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="14">
+      <c r="D9" s="11"/>
+      <c r="E9" s="16">
         <v>22.9</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="22">
-        <f>C9*E9</f>
+      <c r="F9" s="16"/>
+      <c r="G9" s="8">
+        <f t="shared" si="0"/>
         <v>45.8</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15">
+        <v>4</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="17">
+        <v>12.9</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="8">
+        <f t="shared" si="0"/>
+        <v>51.6</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="16">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11">
+        <v>4</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="16">
         <v>12.9</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="22">
-        <f>C10*E10</f>
-        <v>12.9</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>51.6</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="25">
-        <f>SUM(G4:G10)</f>
-        <v>343.15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J13" s="2"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="9">
+        <f>SUM(G4:G11)</f>
+        <v>453.45000000000005</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I14" s="1"/>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="29">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A12:F12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>